<commit_message>
bsearch rotated search and min
</commit_message>
<xml_diff>
--- a/Solution Book.xlsx
+++ b/Solution Book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pshar169\Desktop\leet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pshar169\Desktop\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED88B0F-C12E-4A36-8B7A-40F57C2D478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F1E75B-C54D-469E-AF15-A8775DAA67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{ECD1A7DF-88F1-4771-B47A-D6D279053661}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{ECD1A7DF-88F1-4771-B47A-D6D279053661}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Data Structure</t>
   </si>
@@ -95,12 +95,42 @@
 3. check if all rows are canceled (if !top&lt;=bot), if yes return false
 4. Run binary search on the selected row </t>
   </si>
+  <si>
+    <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>1. Initialize l, r to 1, max(piles) and res to r or max(piles)
+2. While l &lt;= r:
+	initialize hours = 0 
+	k to mid i.e (l+r)//2
+	iterate on p of piles:
+		add math.ceil(p / k) to hours
+	if hours &lt;= h:
+		init res = min (res, k)
+		shift r to low range		
+	else:
+		shift l to high range
+3. return res</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>1. initialize result to any random element
+2. initialize l and r
+3. While l&lt;=r
+	if nums[l] &lt; nums[r] that means arr is sorted assign res = minimum of res, nums[l] and break
+	inititalize mid and assign res = min(res, nums[m]) (# at some point m and l will be equal)
+	if l &lt;= m, move l pointer to the right
+	else move, move r pointer to the left
+4. return result</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,20 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A022EF-BEC8-455B-9F76-8C8337E88E29}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1">
+    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -518,7 +549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="170.25" customHeight="1">
+    <row r="3" spans="1:4" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -530,6 +561,34 @@
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -546,13 +605,13 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.375" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -560,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="85.5">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>

</xml_diff>